<commit_message>
fixes for the tokenizer, also to run on the full dataset to generate report
</commit_message>
<xml_diff>
--- a/results/full_dataset_with_forms.xlsx
+++ b/results/full_dataset_with_forms.xlsx
@@ -16570,34 +16570,34 @@
     <t>х1</t>
   </si>
   <si>
-    <t>['ну_PART', 'анализ_NOUN', 'американский_ADJ', 'военный_ADJ', 'аналитик_NOUN', 'доступный_ADJ', 'публично_ADV', 'это_PRON ', 'более_ADV', 'чем_SCONJ', 'смехотворность_NOUN', 'читать_VERB', 'намедни_ADV', 'парочка_NOUN', 'от_ADP', 'душа_NOUN', 'посмеяться_VERB']</t>
-  </si>
-  <si>
-    <t>['ну_PART', 'в_ADP', 'сравнение_NOUN', 'с_ADP', 'сша_NOUN', 'где_ADV', 'бюджет_NOUN', 'военка_NOUN', 'больше_ADV', 'чем_SCONJ', 'планета_NOUN', 'то_PRON ', 'конечно_ADV', 'а_SCONJ', 'то_PRON ', 'что_SCONJ', 'давать_VERB', 'просраться_VERB', 'весь_DET', 'и_SCONJ', 'сша_NOUN', 'не_PART', 'смочь_VERB', 'после_ADP', 'платить_VERB', 'свой_DET', 'военный_ADJ', 'к_ADP', 'гадалка_NOUN', 'не_PART', 'ходить_VERB']</t>
-  </si>
-  <si>
-    <t>['этот_DET', 'желтуха_NOUN', 'скоро_ADV', 'всерьез_ADV', 'никто_PRON ', 'воспринимать_VERB', 'не_PART', 'будет_ADV']</t>
-  </si>
-  <si>
-    <t>['виталий_NOUN', 'и_SCONJ', 'как_SCONJ', 'там_ADV', 'с_ADP', 'сша_NOUN', 'с_ADP', 'диван_NOUN', 'воюется_VERB']</t>
-  </si>
-  <si>
-    <t>['даже_PART', 'если_SCONJ', 'тысячный_ADJ', 'часть_NOUN', 'доставать_VERB', 'до_ADP', 'пиндосия_NOUN', 'взлетать_VERB', 'он_PRON ', 'мало_ADV', 'не_PART', 'показываться_VERB', 'пусть_PART', 'утешаться_VERB', 'газетка_NOUN']</t>
-  </si>
-  <si>
-    <t>['российский_ADJ', 'армия_NOUN', 'весь_DET', 'сильный_ADJ']</t>
-  </si>
-  <si>
-    <t>['после_ADP', 'слово_NOUN', 'о_ADP', 'нападение_NOUN', 'на_ADP', 'грузия_NOUN', 'переставать_VERB', 'читать_VERB', 'что_SCONJ', 'они_PRON ', 'перед_ADP', 'этот_DET', 'расхерачить_VERB', 'цхенвал_NOUN', 'и_SCONJ', 'российский_ADJ', 'миротворец_NOUN', 'это_PRON ', 'пох_NOUN', 'вот_PART', 'же_PART', 'рашка_NOUN', 'парашка_NOUN', 'то_PRON ', 'на_ADP', 'германия_NOUN', 'нападать_VERB', 'в_ADP', 'то_PRON ', 'на_ADP', 'грузия_NOUN', 'в_ADP', 'агрессор_NOUN', 'эдакий_DET']</t>
-  </si>
-  <si>
-    <t>['руслан_NOUN', 'причем_SCONJ', 'нападение_NOUN', 'грызун_NOUN', 'на_ADP', 'осетия_NOUN', 'являться_VERB', 'известный_ADJ', 'весь_DET', 'мир_NOUN', 'факт_NOUN']</t>
-  </si>
-  <si>
-    <t>['александр_NOUN', 'а_SCONJ', 'че_NOUN', 'кто_PRON ', 'то_PRON ', 'воевать_VERB', 'с_ADP', 'диван_NOUN', 'ты_PRON ', 'мысль_NOUN', 'то_PRON ', 'развивать_VERB', 'учиться_VERB']</t>
-  </si>
-  <si>
-    <t>['григорий_NOUN', 'как_SCONJ', 'видно_ADV', 'в_ADP', 'статья_NOUN', 'не_PART', 'весь_DET', 'мир_NOUN', 'далеко_ADV', 'этот_DET', 'факт_NOUN', 'известный_ADJ', 'и_SCONJ', 'некоторый_DET', 'выгодно_ADV', 'чтобы_SCONJ', 'этот_DET', 'факт_NOUN', 'вообще_ADV', 'быть_VERB', 'забывать_VERB', 'главное_ADV', 'что_SCONJ', 'россия_NOUN', 'войско_NOUN', 'применять_VERB', 'почему_ADV', 'это_PRON ', 'происходить_VERB', 'весь_DET', 'должно_ADV', 'быть_VERB', 'пох_NOUN', 'делать_VERB', 'из_ADP', 'народ_NOUN', 'свой_DET', 'даун_NOUN', 'я_PRON ', 'даже_PART', 'жалко_ADV', 'американец_NOUN', 'обычный_ADJ', 'немного_ADV']</t>
+    <t>ну_PART анализ_NOUN американский_ADJ военный_ADJ аналитик_NOUN доступный_ADJ публично_ADV это_PRON  более_ADV чем_SCONJ смехотворность_NOUN читать_VERB намедни_ADV парочка_NOUN от_ADP душа_NOUN посмеяться_VERB</t>
+  </si>
+  <si>
+    <t>ну_PART в_ADP сравнение_NOUN с_ADP сша_NOUN где_ADV бюджет_NOUN военка_NOUN больше_ADV чем_SCONJ планета_NOUN то_PRON  конечно_ADV а_SCONJ то_PRON  что_SCONJ давать_VERB просраться_VERB весь_DET и_SCONJ сша_NOUN не_PART смочь_VERB после_ADP платить_VERB свой_DET военный_ADJ к_ADP гадалка_NOUN не_PART ходить_VERB</t>
+  </si>
+  <si>
+    <t>этот_DET желтуха_NOUN скоро_ADV всерьез_ADV никто_PRON  воспринимать_VERB не_PART будет_ADV</t>
+  </si>
+  <si>
+    <t>виталий_NOUN и_SCONJ как_SCONJ там_ADV с_ADP сша_NOUN с_ADP диван_NOUN воюется_VERB</t>
+  </si>
+  <si>
+    <t>даже_PART если_SCONJ тысячный_ADJ часть_NOUN доставать_VERB до_ADP пиндосия_NOUN взлетать_VERB он_PRON  мало_ADV не_PART показываться_VERB пусть_PART утешаться_VERB газетка_NOUN</t>
+  </si>
+  <si>
+    <t>российский_ADJ армия_NOUN весь_DET сильный_ADJ</t>
+  </si>
+  <si>
+    <t>после_ADP слово_NOUN о_ADP нападение_NOUN на_ADP грузия_NOUN переставать_VERB читать_VERB что_SCONJ они_PRON  перед_ADP этот_DET расхерачить_VERB цхенвал_NOUN и_SCONJ российский_ADJ миротворец_NOUN это_PRON  пох_NOUN вот_PART же_PART рашка_NOUN парашка_NOUN то_PRON  на_ADP германия_NOUN нападать_VERB в_ADP то_PRON  на_ADP грузия_NOUN в_ADP агрессор_NOUN эдакий_DET</t>
+  </si>
+  <si>
+    <t>руслан_NOUN причем_SCONJ нападение_NOUN грызун_NOUN на_ADP осетия_NOUN являться_VERB известный_ADJ весь_DET мир_NOUN факт_NOUN</t>
+  </si>
+  <si>
+    <t>александр_NOUN а_SCONJ че_NOUN кто_PRON  то_PRON  воевать_VERB с_ADP диван_NOUN ты_PRON  мысль_NOUN то_PRON  развивать_VERB учиться_VERB</t>
+  </si>
+  <si>
+    <t>григорий_NOUN как_SCONJ видно_ADV в_ADP статья_NOUN не_PART весь_DET мир_NOUN далеко_ADV этот_DET факт_NOUN известный_ADJ и_SCONJ некоторый_DET выгодно_ADV чтобы_SCONJ этот_DET факт_NOUN вообще_ADV быть_VERB забывать_VERB главное_ADV что_SCONJ россия_NOUN войско_NOUN применять_VERB почему_ADV это_PRON  происходить_VERB весь_DET должно_ADV быть_VERB пох_NOUN делать_VERB из_ADP народ_NOUN свой_DET даун_NOUN я_PRON  даже_PART жалко_ADV американец_NOUN обычный_ADJ немного_ADV</t>
   </si>
 </sst>
 </file>

</xml_diff>